<commit_message>
adding ack in open ehr importer changes
</commit_message>
<xml_diff>
--- a/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/GEL_openEHR_Cross_references_test.xlsx
+++ b/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/GEL_openEHR_Cross_references_test.xlsx
@@ -1,35 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmilward/Operations/AWS/NorthThames/OpenEhr/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="-20940" windowWidth="32540" windowHeight="18180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="24" r:id="rId1"/>
     <sheet name="RD-Phenotype" sheetId="23" r:id="rId2"/>
     <sheet name="RD-Pedigree" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Full Name of Responsible Consultant (12774.4)</t>
   </si>
@@ -135,6 +130,30 @@
   </si>
   <si>
     <t>Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genomics England Model </t>
+  </si>
+  <si>
+    <t>Rare Disease</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/catalogue/dataModel/37459@1.4.0</t>
+  </si>
+  <si>
+    <t>RD complete except Investigations</t>
+  </si>
+  <si>
+    <t>RD Investigations complete to row 266</t>
+  </si>
+  <si>
+    <t>RD sections complete</t>
+  </si>
+  <si>
+    <t>Cancer withdrawal, disease update, risk factors complete</t>
+  </si>
+  <si>
+    <t>Cancer complete</t>
   </si>
 </sst>
 </file>
@@ -209,7 +228,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -235,8 +254,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -253,20 +273,34 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="25" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -291,6 +325,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -346,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -381,7 +416,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -558,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,75 +603,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="51" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="12.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="51" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="5" spans="1:3">
+      <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B5" s="14">
         <v>42914</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
+      <c r="C5" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>42978</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14">
+        <v>43010</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="13">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14">
+        <v>43013</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="13">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14">
+        <v>43031</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -648,7 +738,7 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="39.83203125" style="3" customWidth="1"/>
@@ -657,7 +747,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -669,7 +759,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80">
       <c r="A2" s="3">
         <v>12502.2</v>
       </c>
@@ -680,7 +770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="80">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -691,7 +781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="80">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -702,9 +792,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:4" ht="17" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -712,11 +807,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD53"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.5" style="2" customWidth="1"/>
@@ -725,7 +820,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -737,7 +832,7 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="75">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -749,7 +844,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="80">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -761,7 +856,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="80">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -773,7 +868,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="80">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -785,7 +880,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -799,5 +894,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
addding open ehr stuff back in
</commit_message>
<xml_diff>
--- a/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/GEL_openEHR_Cross_references_test.xlsx
+++ b/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/GEL_openEHR_Cross_references_test.xlsx
@@ -153,7 +153,7 @@
     <t>Cancer complete</t>
   </si>
   <si>
-    <t>http://localhost:8080/catalogue/dataModel/15000000@1.4.0</t>
+    <t>http://localhost:8080/catalogue/dataModel/15000000</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -727,7 +727,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="http://localhost:8080/catalogue/dataModel/37459@1.4.0"/>
+    <hyperlink ref="C1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>